<commit_message>
Pause work on CSV; commit changes thus far
</commit_message>
<xml_diff>
--- a/Excavator.CSV/SampleData.xlsx
+++ b/Excavator.CSV/SampleData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>FamilyName</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>EmailIsActive</t>
-  </si>
-  <si>
     <t>RecordType</t>
   </si>
   <si>
@@ -80,12 +77,6 @@
     <t>FirstVisit</t>
   </si>
   <si>
-    <t>Address1</t>
-  </si>
-  <si>
-    <t>Address2</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
@@ -189,6 +180,39 @@
   </si>
   <si>
     <t>cindy@rocksoliddemochurch.com</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>Suffix</t>
+  </si>
+  <si>
+    <t>IsEmailActive</t>
+  </si>
+  <si>
+    <t>Campus</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Street1</t>
+  </si>
+  <si>
+    <t>Street2</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>PreviousChurch</t>
+  </si>
+  <si>
+    <t>Custom2</t>
   </si>
 </sst>
 </file>
@@ -196,8 +220,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -254,16 +278,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -550,11 +574,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AM3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,304 +588,315 @@
     <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="1"/>
-    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" style="1" customWidth="1"/>
+    <col min="20" max="21" width="13.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="1"/>
+    <col min="25" max="25" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AG1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>29</v>
+      <c r="AM1" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1">
         <f>1+1</f>
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="K2" s="5">
+        <v>27800</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="5">
-        <v>27800</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="R2" s="1">
+        <v>6235553322</v>
+      </c>
+      <c r="S2" s="1">
+        <v>6235553322</v>
+      </c>
+      <c r="T2" s="1">
+        <v>6025552911</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2" s="1">
-        <v>6235553322</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>6235553322</v>
-      </c>
-      <c r="R2" s="1">
-        <v>6025552911</v>
-      </c>
-      <c r="S2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>85029</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC2" s="7">
+        <v>33.593043000000002</v>
+      </c>
+      <c r="AD2" s="7">
+        <v>-112.126518</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>37147</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>41258</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="X2" s="1">
-        <v>85029</v>
-      </c>
-      <c r="Y2" s="7">
-        <v>33.593043000000002</v>
-      </c>
-      <c r="Z2" s="7">
-        <v>-112.126518</v>
-      </c>
-      <c r="AB2" s="5">
-        <v>37147</v>
-      </c>
-      <c r="AC2" s="5">
-        <v>41258</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1">
         <f>C2+1</f>
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="K3" s="5">
+        <v>28194</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="5">
-        <v>28194</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q3" s="1">
+      <c r="S3" s="1">
         <v>6392849127</v>
       </c>
-      <c r="AC3" s="5">
+      <c r="AG3" s="5">
         <v>37147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="10">
+  <dataValidations count="11">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unique ID Verification" prompt="ID must be unique and greater than 1." sqref="C2:C1048576">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Gender Required" promptTitle="Gender Required" sqref="J1:J1048576">
+    <dataValidation type="list" allowBlank="1" errorTitle="Gender Required" promptTitle="Gender Required" sqref="L1:L1048576">
       <formula1>"Male,Female,Unknown"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" errorTitle="RecordType Required" promptTitle="RecordType Required" sqref="D1:D1048576">
@@ -870,28 +905,29 @@
     <dataValidation type="list" allowBlank="1" errorTitle="RecordStatus Required" promptTitle="RecordStatus Required" sqref="E1:E1048576">
       <formula1>"Active,Inactive,Pending"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="EmailIsActive Required" promptTitle="EmailIsActive Required" sqref="L1:L1048576">
+    <dataValidation type="list" allowBlank="1" errorTitle="EmailIsActive Required" promptTitle="EmailIsActive Required" sqref="N1:N1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="M1:M1048576">
+    <dataValidation type="list" allowBlank="1" sqref="O1:O1048576">
       <formula1>"Attendee,Member,Visitor,Web Prospect,Participant"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="N1:N1048576">
+    <dataValidation type="list" allowBlank="1" sqref="P1:P1048576">
       <formula1>"Married,Single,Unknown"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="O1:O1048576">
+    <dataValidation type="list" allowBlank="1" sqref="Q1:Q1048576">
       <formula1>"Adult,Child"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" sqref="P1:R1048576">
+    <dataValidation type="whole" allowBlank="1" sqref="R1:U1048576">
       <formula1>1111111111</formula1>
       <formula2>9999999999</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="S1:S1048576">
+    <dataValidation type="list" allowBlank="1" sqref="V1:V1048576">
       <formula1>"Home,Work,Previous,Meeting Location"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" errorTitle="RecordStatus Required" promptTitle="RecordStatus Required" sqref="F1:F1048576"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1"/>
+    <hyperlink ref="M3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>